<commit_message>
Revert "Merge branch 'main' of https://github.com/WhiteNightD/CatClub"
This reverts commit c95e28d3aa39f7aa726a6a7b3d251453c83be496, reversing
changes made to 4db86908b915ab81b497a7683a954d93327c79bb.
</commit_message>
<xml_diff>
--- a/ExcelConfig/pbjson/excel/应用效果表.xlsx
+++ b/ExcelConfig/pbjson/excel/应用效果表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CatClub\ExcelConfig\pbjson\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4671D3F0-6A29-4C9C-82B4-AD5FE8FEE3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953044BD-C057-4582-8987-0465FD095B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="3450" windowWidth="25800" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11085" yWindow="4650" windowWidth="25800" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#应用效果表" sheetId="1" r:id="rId1"/>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F443"/>
+  <dimension ref="A1:F442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="C439" sqref="C439"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6409,17 +6409,6 @@
       </c>
       <c r="E442" s="2"/>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A443" s="2">
-        <v>540139</v>
-      </c>
-      <c r="B443" s="3">
-        <v>5302</v>
-      </c>
-      <c r="C443" s="4"/>
-      <c r="D443" s="5"/>
-      <c r="E443" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>